<commit_message>
feature: update system solder
</commit_message>
<xml_diff>
--- a/equipment_sequence/lin_zhong/system_solder/system_solder_manual_20250616_new.xlsx
+++ b/equipment_sequence/lin_zhong/system_solder/system_solder_manual_20250616_new.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17775" tabRatio="530" firstSheet="2" activeTab="3"/>
+    <workbookView windowWidth="27945" windowHeight="12375" tabRatio="530" firstSheet="2" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="secs指令" sheetId="14" r:id="rId1"/>
@@ -5249,10 +5249,10 @@
   <sheetPr/>
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18:B28"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -6787,7 +6787,7 @@
   <sheetPr/>
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
@@ -6847,7 +6847,7 @@
       </c>
       <c r="E3" s="94"/>
     </row>
-    <row r="4" ht="37.5" spans="1:5">
+    <row r="4" ht="18.75" spans="1:5">
       <c r="A4" s="96">
         <v>608</v>
       </c>

</xml_diff>